<commit_message>
add asignatura to user schema
</commit_message>
<xml_diff>
--- a/public/plantilla excel/plantilla de excel.xlsx
+++ b/public/plantilla excel/plantilla de excel.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Nombre</t>
   </si>
@@ -29,12 +29,15 @@
   <si>
     <t>Curso</t>
   </si>
+  <si>
+    <t>Asignatura</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -44,7 +47,10 @@
     <font>
       <color theme="1"/>
       <name val="Aptos narrow"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -67,11 +73,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -293,7 +302,7 @@
     <col customWidth="1" min="3" max="3" width="21.13"/>
     <col customWidth="1" min="4" max="4" width="22.88"/>
     <col customWidth="1" min="5" max="5" width="20.0"/>
-    <col customWidth="1" min="6" max="26" width="8.63"/>
+    <col customWidth="1" min="6" max="6" width="14.88"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -311,6 +320,9 @@
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>

</xml_diff>